<commit_message>
Add support for file path in cell and support paths starting with / or starting with project name
</commit_message>
<xml_diff>
--- a/storage/test_data/etl/file_associations.xlsx
+++ b/storage/test_data/etl/file_associations.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">S:bead width (mm)</t>
   </si>
   <si>
-    <t xml:space="preserve">FILE:File that exists:P1/D1</t>
+    <t xml:space="preserve">FILE:File that exists</t>
   </si>
   <si>
     <t xml:space="preserve">File: File that doesn’t exist:P1</t>
@@ -64,13 +64,16 @@
     <t xml:space="preserve">file:/</t>
   </si>
   <si>
+    <t xml:space="preserve">file:</t>
+  </si>
+  <si>
     <t xml:space="preserve">G181030g</t>
   </si>
   <si>
     <t xml:space="preserve">Ti-6Al-4V</t>
   </si>
   <si>
-    <t xml:space="preserve">f1.txt</t>
+    <t xml:space="preserve">P1/D1/f1.txt</t>
   </si>
   <si>
     <t xml:space="preserve">does-not-exist.txt</t>
@@ -83,6 +86,29 @@
   </si>
   <si>
     <t xml:space="preserve">f4.txt</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/D1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">/f5.txt</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -92,7 +118,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -114,6 +140,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -158,13 +192,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="75" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -189,7 +227,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="M6" activeCellId="0" sqref="M6"/>
+      <selection pane="bottomLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -254,6 +292,9 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="ALT1" s="0"/>
       <c r="ALU1" s="0"/>
       <c r="ALV1" s="0"/>
@@ -274,7 +315,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>1</v>
@@ -283,7 +324,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>1.6</v>
@@ -293,22 +334,25 @@
       </c>
       <c r="I2" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>118.405161455004</v>
+        <v>120.8514608769</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Test and fixes to handle relative paths with a path specified in the header
</commit_message>
<xml_diff>
--- a/storage/test_data/etl/file_associations.xlsx
+++ b/storage/test_data/etl/file_associations.xlsx
@@ -49,7 +49,7 @@
     <t xml:space="preserve">S:bead width (mm)</t>
   </si>
   <si>
-    <t xml:space="preserve">FILE:File that exists</t>
+    <t xml:space="preserve">FILE:File that exists:</t>
   </si>
   <si>
     <t xml:space="preserve">File: File that doesn’t exist:P1</t>
@@ -218,19 +218,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="O2" activeCellId="0" sqref="O2"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.0078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.15"/>
@@ -245,8 +245,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="19.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="13.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="13" style="0" width="8.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="17" style="0" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="10.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="10.5"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="132" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -334,7 +333,7 @@
       </c>
       <c r="I2" s="0" t="n">
         <f aca="true">RAND()*50 + 100</f>
-        <v>120.8514608769</v>
+        <v>105.8180356477</v>
       </c>
       <c r="J2" s="0" t="s">
         <v>17</v>
@@ -367,14 +366,13 @@
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J1" r:id="rId1" display="FILE:File that exists"/>
-    <hyperlink ref="L1" r:id="rId2" display="File:that exists with path:P1/D1"/>
-    <hyperlink ref="M1" r:id="rId3" display="file:P1/D1"/>
-    <hyperlink ref="N1" r:id="rId4" display="file:/"/>
+    <hyperlink ref="L1" r:id="rId1" display="File:that exists with path:P1/D1"/>
+    <hyperlink ref="M1" r:id="rId2" display="file:P1/D1"/>
+    <hyperlink ref="N1" r:id="rId3" display="file:/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>